<commit_message>
new plan for review
</commit_message>
<xml_diff>
--- a/Time Plan.xlsx
+++ b/Time Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJJ\Desktop\MaxBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2667BF47-C4F3-49A1-9B08-A72FBE6A0C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AB53B5-19B7-48C3-9069-326899F89141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3744" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>AEM Exam</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,6 +104,14 @@
   </si>
   <si>
     <t>PEAC Q&amp;A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AEM PDE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AEM PCA &amp; PDE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -114,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +146,19 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -159,10 +180,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -445,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -463,41 +487,41 @@
     <col min="37" max="40" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3">
         <v>44183</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>44184</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>44185</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>44186</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -506,7 +530,7 @@
         <v>44187</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -517,7 +541,10 @@
         <v>44188</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,13 +554,16 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44190</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>